<commit_message>
Updated smt results and added figures
</commit_message>
<xml_diff>
--- a/TACO2019.xlsx
+++ b/TACO2019.xlsx
@@ -3,17 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="231" documentId="11_F25DC773A252ABEACE02ECA5E39F7D7C5ADE589E" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{D1D6361E-C373-4ACF-B11E-3B71FFFE3F0B}"/>
+  <xr:revisionPtr revIDLastSave="297" documentId="11_F25DC773A252ABEACE02ECA5E39F7D7C5ADE589E" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{FB162791-A490-46CA-8E8A-C2BA9E53BFB8}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fig-elpase-time" sheetId="2" r:id="rId1"/>
-    <sheet name="fig-data-tlb-under-code-superpg" sheetId="3" r:id="rId2"/>
-    <sheet name="data-superpg" sheetId="1" r:id="rId3"/>
+    <sheet name="fig-dtlb-code-sup-data-nosup" sheetId="3" r:id="rId2"/>
+    <sheet name="fig-dlb-code-sup-data-sup" sheetId="4" r:id="rId3"/>
+    <sheet name="data-superpg" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="32">
   <si>
     <t>Intel Skylake processor</t>
   </si>
@@ -109,7 +109,22 @@
     <t>code superpage, data no superpage / code no superpagge, data no superpage</t>
   </si>
   <si>
-    <t>code superpage, data superpage / code no sueprpage, data superpage</t>
+    <t>code w/o superpg, data w/t superpg</t>
+  </si>
+  <si>
+    <t>code w/t superpg, data w/o superpg</t>
+  </si>
+  <si>
+    <t>code w/t superpg, data w/t superpg</t>
+  </si>
+  <si>
+    <t>normalized to data no superpg</t>
+  </si>
+  <si>
+    <t>normalized to data superpg</t>
+  </si>
+  <si>
+    <t>code superpage, data superpage / code no superpagge, data superpage</t>
   </si>
 </sst>
 </file>
@@ -245,7 +260,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> code no superpage, data superpage </c:v>
+                  <c:v> code w/o superpg, data w/t superpg </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -301,10 +316,10 @@
                   <c:v>0.59111913452409148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95962310781587901</c:v>
+                  <c:v>0.95834018377450181</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.95962310781587901</c:v>
+                  <c:v>0.94317910192931542</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.0001952633578108</c:v>
@@ -330,7 +345,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> code superpage, data no superpage </c:v>
+                  <c:v> code w/t superpg, data w/o superpg </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -386,10 +401,10 @@
                   <c:v>0.98373537877238537</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9887007447959768</c:v>
+                  <c:v>0.96440947487430251</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9887007447959768</c:v>
+                  <c:v>0.99642857142857144</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.98628202051916747</c:v>
@@ -415,7 +430,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> code superpage, data superpage </c:v>
+                  <c:v> code w/t superpg, data w/t superpg </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -471,10 +486,10 @@
                   <c:v>0.56374615812400097</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9526365180909856</c:v>
+                  <c:v>0.94043884337522177</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9526365180909856</c:v>
+                  <c:v>0.94227817009517967</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.98533241886613199</c:v>
@@ -584,7 +599,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -597,22 +612,22 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:rPr lang="en-US" sz="2000" b="1"/>
                   <a:t>Normalized</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                  <a:rPr lang="en-US" sz="2000" b="1" baseline="0"/>
                   <a:t> </a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:rPr lang="en-US" sz="2000" b="1"/>
                   <a:t>Elapse</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                  <a:rPr lang="en-US" sz="2000" b="1" baseline="0"/>
                   <a:t> Time</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="2000"/>
+                <a:endParaRPr lang="en-US" sz="2000" b="1"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -637,7 +652,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -702,10 +717,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.24247755749419886"/>
+          <c:x val="1.6643780760874399E-2"/>
           <c:y val="0.64654368793085637"/>
-          <c:w val="0.61764637316941218"/>
-          <c:h val="0.17977005096726487"/>
+          <c:w val="0.96959511576434765"/>
+          <c:h val="0.10504456653971232"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -861,16 +876,16 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.93739559102557135</c:v>
+                  <c:v>0.51541159723365515</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.9725114905184209</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.70296576895721952</c:v>
+                  <c:v>0.74256563675374176</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9488834135343307</c:v>
+                  <c:v>0.92959391410953796</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.95189771697377712</c:v>
@@ -884,91 +899,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-EB53-4DA9-834E-1FA34604E180}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'data-superpg'!$C$71</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v> code superpage, data superpage / code no sueprpage, data superpage </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'data-superpg'!$A$72:$A$77</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Clang</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>PostgreSQL</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Javac</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Derby</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Node.js</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>MySQL</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'data-superpg'!$C$72:$C$77</c:f>
-              <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.9334557455450897</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.98361426054840106</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.87869444641081806</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.68539774451855962</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.91413733839426947</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.72003049098828042</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-EB53-4DA9-834E-1FA34604E180}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -980,7 +910,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="300"/>
+        <c:gapWidth val="400"/>
         <c:overlap val="-27"/>
         <c:axId val="934866728"/>
         <c:axId val="934860496"/>
@@ -1065,7 +995,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1078,23 +1008,23 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" b="1"/>
                   <a:t>Normalized</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" b="1" baseline="0"/>
                   <a:t> Data Page </a:t>
                 </a:r>
               </a:p>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr b="1"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t>Table Walking Cycles</a:t>
+                  <a:rPr lang="en-US" b="1" baseline="0"/>
+                  <a:t>Table Walk Cycles</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" b="1"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1119,7 +1049,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1178,19 +1108,352 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="2000"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
       <c:layout>
         <c:manualLayout>
+          <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="1.2364950578051224E-2"/>
-          <c:y val="0.76402585733936568"/>
-          <c:w val="0.9876350494219488"/>
-          <c:h val="0.11883689680122766"/>
+          <c:x val="0.18688903466091539"/>
+          <c:y val="3.475235952197317E-2"/>
+          <c:w val="0.79698858946637574"/>
+          <c:h val="0.51799883912314038"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'data-superpg'!$B$81</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> code superpage, data superpage / code no superpagge, data superpage </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'data-superpg'!$A$72:$A$77</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Clang</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PostgreSQL</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Javac</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Derby</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Node.js</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MySQL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'data-superpg'!$B$82:$B$87</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.49154000020318295</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98361426054840106</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90431492898636334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.51917900623807023</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.91413733839426947</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.72003049098828042</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-101E-4031-994E-133569B25241}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="400"/>
+        <c:overlap val="-27"/>
+        <c:axId val="934866728"/>
+        <c:axId val="934860496"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="934866728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="934860496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="934860496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Normalized</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0"/>
+                  <a:t> Data Page </a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0"/>
+                  <a:t>Table Walk Cycles</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.9302880931233973E-2"/>
+              <c:y val="0.13568710393028377"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="934866728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1198,27 +1461,7 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1333,6 +1576,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1837,6 +2120,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2346,7 +3132,8 @@
     <sheetView zoomScale="103" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -2354,10 +3141,23 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{35D17F88-6A46-4034-9011-E7AA1015A24A}">
   <sheetPr/>
   <sheetViews>
+    <sheetView zoomScale="103" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{81477436-2C6E-4FA7-9190-7774881B2D35}">
+  <sheetPr/>
+  <sheetViews>
     <sheetView tabSelected="1" zoomScale="103" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -2405,6 +3205,39 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D62C6D47-F9D5-4409-BA05-CA7617829327}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8660352" cy="6288350"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7C5DD54-A6A1-4762-8D2E-D95B955CB578}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2690,10 +3523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L77"/>
+  <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72:C72"/>
+    <sheetView topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2746,32 +3579,32 @@
         <v>5</v>
       </c>
       <c r="B5" s="3">
-        <v>2674726.7326000002</v>
+        <v>1585133.47765</v>
       </c>
       <c r="C5" s="3">
-        <v>2690581.50055</v>
+        <v>1620427.36555</v>
       </c>
       <c r="D5" s="3">
-        <v>193823.9283</v>
+        <v>656908.25349999999</v>
       </c>
       <c r="E5" s="3">
-        <v>148097.10935000001</v>
+        <v>646197.75254999998</v>
       </c>
       <c r="I5" s="3">
         <f>C5/B5</f>
-        <v>1.0059276215984083</v>
+        <v>1.022265562110469</v>
       </c>
       <c r="J5" s="3">
         <f>D5/B5</f>
-        <v>7.2464946021454354E-2</v>
+        <v>0.41441825736586102</v>
       </c>
       <c r="K5" s="3">
         <f>E5/B5</f>
-        <v>5.5369061648417608E-2</v>
+        <v>0.40766141253164639</v>
       </c>
       <c r="L5" s="3">
         <f>E5/C5</f>
-        <v>5.5042788824544615E-2</v>
+        <v>0.39878230045236845</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
@@ -2779,32 +3612,32 @@
         <v>6</v>
       </c>
       <c r="B6" s="3">
-        <v>269532641.56809998</v>
+        <v>538604.22155000002</v>
       </c>
       <c r="C6" s="3">
-        <v>270569085.08074999</v>
+        <v>550671.14994999999</v>
       </c>
       <c r="D6" s="3">
-        <v>254972162.96145001</v>
+        <v>437690.78615</v>
       </c>
       <c r="E6" s="3">
-        <v>254927708.68669999</v>
+        <v>420984.0122</v>
       </c>
       <c r="I6" s="3">
         <f>C6/B6</f>
-        <v>1.0038453357879777</v>
+        <v>1.0224040731899087</v>
       </c>
       <c r="J6" s="3">
         <f>D6/B6</f>
-        <v>0.94597879306217125</v>
+        <v>0.81263898171909899</v>
       </c>
       <c r="K6" s="3">
         <f>E6/B6</f>
-        <v>0.94581386211172525</v>
+        <v>0.78162033522219421</v>
       </c>
       <c r="L6" s="3">
         <f>E6/C6</f>
-        <v>0.94219082202468951</v>
+        <v>0.76449258734223613</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
@@ -2813,35 +3646,35 @@
       </c>
       <c r="B7" s="4">
         <f>B5+B6</f>
-        <v>272207368.30069995</v>
+        <v>2123737.6992000001</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" ref="C7:E7" si="0">C5+C6</f>
-        <v>273259666.58129996</v>
+        <v>2171098.5154999997</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" si="0"/>
-        <v>255165986.88975</v>
+        <v>1094599.0396499999</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>255075805.79604998</v>
+        <v>1067181.7647500001</v>
       </c>
       <c r="I7" s="3">
         <f>C7/B7</f>
-        <v>1.0038657964594022</v>
+        <v>1.0223006901077474</v>
       </c>
       <c r="J7" s="3">
         <f>D7/B7</f>
-        <v>0.93739559102557135</v>
+        <v>0.51541159723365515</v>
       </c>
       <c r="K7" s="3">
         <f>E7/B7</f>
-        <v>0.93706429546122649</v>
+        <v>0.50250168142327623</v>
       </c>
       <c r="L7" s="3">
         <f>E7/C7</f>
-        <v>0.9334557455450897</v>
+        <v>0.49154000020318295</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
@@ -2849,32 +3682,32 @@
         <v>17</v>
       </c>
       <c r="B8" s="3">
-        <v>1585133.47765</v>
+        <v>2674726.7326000002</v>
       </c>
       <c r="C8" s="3">
-        <v>1620427.36555</v>
+        <v>2690581.50055</v>
       </c>
       <c r="D8" s="3">
-        <v>656908.25349999999</v>
+        <v>193823.9283</v>
       </c>
       <c r="E8" s="3">
-        <v>646197.75254999998</v>
+        <v>148097.10935000001</v>
       </c>
       <c r="I8" s="3">
         <f>C8/B8</f>
-        <v>1.022265562110469</v>
+        <v>1.0059276215984083</v>
       </c>
       <c r="J8" s="3">
         <f>D8/B8</f>
-        <v>0.41441825736586102</v>
+        <v>7.2464946021454354E-2</v>
       </c>
       <c r="K8" s="3">
         <f>E8/B8</f>
-        <v>0.40766141253164639</v>
+        <v>5.5369061648417608E-2</v>
       </c>
       <c r="L8" s="3">
         <f>E8/C8</f>
-        <v>0.39878230045236845</v>
+        <v>5.5042788824544615E-2</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
@@ -2905,10 +3738,6 @@
         <f>E9/B9</f>
         <v>0.92242822567088012</v>
       </c>
-      <c r="L9" s="3">
-        <f>E9/C9</f>
-        <v>0.91897869333498516</v>
-      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
@@ -3058,16 +3887,16 @@
         <v>5</v>
       </c>
       <c r="B23" s="3">
-        <v>20877943.837000001</v>
+        <v>40715831.067000002</v>
       </c>
       <c r="C23" s="3">
-        <v>4515750.8480000002</v>
+        <v>8688710.7245000005</v>
       </c>
       <c r="D23" s="3">
-        <v>14619384.566</v>
+        <v>30202759.653499998</v>
       </c>
       <c r="E23" s="3">
-        <v>4030061.1965000001</v>
+        <v>7973910.0724999998</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
@@ -3075,16 +3904,16 @@
         <v>6</v>
       </c>
       <c r="B24" s="3">
-        <v>984439.28700000001</v>
+        <v>1871091.513</v>
       </c>
       <c r="C24" s="3">
-        <v>336751.87</v>
+        <v>653553.84750000003</v>
       </c>
       <c r="D24" s="3">
-        <v>749122.39800000004</v>
+        <v>1420825.6295</v>
       </c>
       <c r="E24" s="3">
-        <v>233805.99299999999</v>
+        <v>474439.25050000002</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
@@ -3093,35 +3922,35 @@
       </c>
       <c r="B25" s="4">
         <f>B23+B24</f>
-        <v>21862383.124000002</v>
+        <v>42586922.579999998</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" ref="C25:E25" si="2">C23+C24</f>
-        <v>4852502.7180000003</v>
+        <v>9342264.5720000006</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" si="2"/>
-        <v>15368506.964</v>
+        <v>31623585.283</v>
       </c>
       <c r="E25" s="4">
         <f t="shared" si="2"/>
-        <v>4263867.1895000003</v>
+        <v>8448349.3229999989</v>
       </c>
       <c r="I25" s="3">
         <f>C25/B25</f>
-        <v>0.22195671398115052</v>
+        <v>0.21936932762517541</v>
       </c>
       <c r="J25" s="3">
         <f>D25/B25</f>
-        <v>0.70296576895721952</v>
+        <v>0.74256563675374176</v>
       </c>
       <c r="K25" s="3">
         <f>E25/B25</f>
-        <v>0.19503213191883134</v>
+        <v>0.1983789579331468</v>
       </c>
       <c r="L25" s="3">
         <f>E25/C25</f>
-        <v>0.87869444641081806</v>
+        <v>0.90431492898636334</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
@@ -3129,32 +3958,32 @@
         <v>17</v>
       </c>
       <c r="B26" s="3">
-        <v>8594040.1539999992</v>
+        <v>16986050.2445</v>
       </c>
       <c r="C26" s="3">
-        <v>3060212.8679999998</v>
+        <v>5764950.7165000001</v>
       </c>
       <c r="D26" s="3">
-        <v>462685.40100000001</v>
+        <v>1180749.4624999999</v>
       </c>
       <c r="E26" s="3">
-        <v>252987.1115</v>
+        <v>332630.49300000002</v>
       </c>
       <c r="I26" s="3">
         <f>C26/B26</f>
-        <v>0.35608547472001956</v>
+        <v>0.33939324525233067</v>
       </c>
       <c r="J26" s="3">
         <f>D26/B26</f>
-        <v>5.3837938002261755E-2</v>
+        <v>6.9512891196252105E-2</v>
       </c>
       <c r="K26" s="3">
         <f>E26/B26</f>
-        <v>2.9437506337720565E-2</v>
+        <v>1.9582568531946037E-2</v>
       </c>
       <c r="L26" s="3">
         <f>E26/C26</f>
-        <v>8.2669775735352544E-2</v>
+        <v>5.7698757432213692E-2</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.45">
@@ -3162,28 +3991,28 @@
         <v>14</v>
       </c>
       <c r="B27" s="3">
-        <v>776.57500000000005</v>
+        <v>524.60500000000002</v>
       </c>
       <c r="C27" s="3">
-        <v>809.25</v>
+        <v>547.41</v>
       </c>
       <c r="D27" s="3">
-        <v>785.45</v>
+        <v>543.96500000000003</v>
       </c>
       <c r="E27" s="3">
-        <v>815.18499999999995</v>
+        <v>557.83000000000004</v>
       </c>
       <c r="I27" s="3">
         <f>B27/C27</f>
-        <v>0.95962310781587901</v>
+        <v>0.95834018377450181</v>
       </c>
       <c r="J27" s="3">
         <f>B27/D27</f>
-        <v>0.9887007447959768</v>
+        <v>0.96440947487430251</v>
       </c>
       <c r="K27" s="3">
         <f>B27/E27</f>
-        <v>0.9526365180909856</v>
+        <v>0.94043884337522177</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.45">
@@ -3196,16 +4025,16 @@
         <v>5</v>
       </c>
       <c r="B32" s="3">
-        <v>47433019.658749998</v>
+        <v>95471868.693124995</v>
       </c>
       <c r="C32" s="3">
-        <v>1619882.3525</v>
+        <v>2867630.5165630002</v>
       </c>
       <c r="D32" s="3">
-        <v>45115197.759999998</v>
+        <v>88783582.809062004</v>
       </c>
       <c r="E32" s="3">
-        <v>1200854.4550000001</v>
+        <v>1521575.1243749999</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
@@ -3213,16 +4042,16 @@
         <v>6</v>
       </c>
       <c r="B33" s="3">
-        <v>1730469.8025</v>
+        <v>3622480.2303129998</v>
       </c>
       <c r="C33" s="3">
-        <v>485031.66499999998</v>
+        <v>984319.51843699999</v>
       </c>
       <c r="D33" s="3">
-        <v>1535221.9412499999</v>
+        <v>3333920.8728129999</v>
       </c>
       <c r="E33" s="3">
-        <v>241848.86499999999</v>
+        <v>478276.46687499998</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
@@ -3231,35 +4060,35 @@
       </c>
       <c r="B34" s="4">
         <f>B32+B33</f>
-        <v>49163489.46125</v>
+        <v>99094348.923437998</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" ref="C34:E34" si="3">C32+C33</f>
-        <v>2104914.0175000001</v>
+        <v>3851950.0350000001</v>
       </c>
       <c r="D34" s="4">
         <f t="shared" si="3"/>
-        <v>46650419.701249994</v>
+        <v>92117503.681875005</v>
       </c>
       <c r="E34" s="4">
         <f t="shared" si="3"/>
-        <v>1442703.32</v>
+        <v>1999851.5912499998</v>
       </c>
       <c r="I34" s="3">
         <f>C34/B34</f>
-        <v>4.2814577251662843E-2</v>
+        <v>3.887154087844185E-2</v>
       </c>
       <c r="J34" s="3">
         <f>D34/B34</f>
-        <v>0.9488834135343307</v>
+        <v>0.92959391410953796</v>
       </c>
       <c r="K34" s="3">
         <f>E34/B34</f>
-        <v>2.9345014680805345E-2</v>
+        <v>2.0181287964211963E-2</v>
       </c>
       <c r="L34" s="3">
         <f>E34/C34</f>
-        <v>0.68539774451855962</v>
+        <v>0.51917900623807023</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
@@ -3267,32 +4096,32 @@
         <v>17</v>
       </c>
       <c r="B35" s="3">
-        <v>5014041.3387500001</v>
+        <v>9583044.796875</v>
       </c>
       <c r="C35" s="3">
-        <v>1239456.130625</v>
+        <v>2362508.3725000001</v>
       </c>
       <c r="D35" s="3">
-        <v>817072.56874999998</v>
+        <v>2914273.7112500002</v>
       </c>
       <c r="E35" s="3">
-        <v>279641.88312499999</v>
+        <v>285642.35499999998</v>
       </c>
       <c r="I35" s="3">
         <f>C35/B35</f>
-        <v>0.24719703067585722</v>
+        <v>0.24653003534642834</v>
       </c>
       <c r="J35" s="3">
         <f>D35/B35</f>
-        <v>0.16295688717909454</v>
+        <v>0.30410728249964308</v>
       </c>
       <c r="K35" s="3">
         <f>E35/B35</f>
-        <v>5.5771754605181349E-2</v>
+        <v>2.980705621799316E-2</v>
       </c>
       <c r="L35" s="3">
         <f>E35/C35</f>
-        <v>0.22561660410198595</v>
+        <v>0.12090638844921171</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.45">
@@ -3300,28 +4129,28 @@
         <v>14</v>
       </c>
       <c r="B36" s="3">
-        <v>776.57500000000005</v>
+        <v>414.315</v>
       </c>
       <c r="C36" s="3">
-        <v>809.25</v>
+        <v>439.27499999999998</v>
       </c>
       <c r="D36" s="3">
-        <v>785.45</v>
+        <v>415.8</v>
       </c>
       <c r="E36" s="3">
-        <v>815.18499999999995</v>
+        <v>439.69499999999999</v>
       </c>
       <c r="I36" s="3">
         <f>B36/C36</f>
-        <v>0.95962310781587901</v>
+        <v>0.94317910192931542</v>
       </c>
       <c r="J36" s="3">
         <f>B36/D36</f>
-        <v>0.9887007447959768</v>
+        <v>0.99642857142857144</v>
       </c>
       <c r="K36" s="3">
         <f>B36/E36</f>
-        <v>0.9526365180909856</v>
+        <v>0.94227817009517967</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.45">
@@ -3600,18 +4429,18 @@
         <v>0.94643140561613248</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="63" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:12" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A60" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.45">
@@ -3646,28 +4475,28 @@
       <c r="A63" t="s">
         <v>8</v>
       </c>
-      <c r="B63" s="4">
-        <v>0.95962310781587901</v>
-      </c>
-      <c r="C63" s="4">
-        <v>0.9887007447959768</v>
-      </c>
-      <c r="D63" s="4">
-        <v>0.9526365180909856</v>
+      <c r="B63" s="3">
+        <v>0.95834018377450181</v>
+      </c>
+      <c r="C63" s="3">
+        <v>0.96440947487430251</v>
+      </c>
+      <c r="D63" s="3">
+        <v>0.94043884337522177</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>10</v>
       </c>
-      <c r="B64" s="4">
-        <v>0.95962310781587901</v>
-      </c>
-      <c r="C64" s="4">
-        <v>0.9887007447959768</v>
-      </c>
-      <c r="D64" s="4">
-        <v>0.9526365180909856</v>
+      <c r="B64" s="3">
+        <v>0.94317910192931542</v>
+      </c>
+      <c r="C64" s="3">
+        <v>0.99642857142857144</v>
+      </c>
+      <c r="D64" s="3">
+        <v>0.94227817009517967</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.45">
@@ -3698,6 +4527,11 @@
         <v>0.94643140561613248</v>
       </c>
     </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="71" spans="1:4" ht="126" x14ac:dyDescent="0.5">
       <c r="A71" s="6" t="s">
         <v>23</v>
@@ -3705,9 +4539,7 @@
       <c r="B71" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.45">
@@ -3715,71 +4547,139 @@
         <v>18</v>
       </c>
       <c r="B72" s="3">
-        <v>0.93739559102557135</v>
-      </c>
-      <c r="C72" s="3">
-        <v>0.9334557455450897</v>
-      </c>
+        <f>$D7/$B7</f>
+        <v>0.51541159723365515</v>
+      </c>
+      <c r="C72" s="3"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>9</v>
       </c>
-      <c r="B73" s="4">
+      <c r="B73" s="3">
+        <f>$D15/$B15</f>
         <v>0.9725114905184209</v>
       </c>
-      <c r="C73" s="4">
-        <v>0.98361426054840106</v>
-      </c>
+      <c r="C73" s="4"/>
       <c r="D73" s="4"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>8</v>
       </c>
-      <c r="B74" s="4">
-        <v>0.70296576895721952</v>
-      </c>
-      <c r="C74" s="4">
-        <v>0.87869444641081806</v>
-      </c>
+      <c r="B74" s="3">
+        <f>$D25/$B25</f>
+        <v>0.74256563675374176</v>
+      </c>
+      <c r="C74" s="4"/>
       <c r="D74" s="4"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>10</v>
       </c>
-      <c r="B75" s="4">
-        <v>0.9488834135343307</v>
-      </c>
-      <c r="C75" s="4">
-        <v>0.68539774451855962</v>
-      </c>
+      <c r="B75" s="3">
+        <f>$D34/$B34</f>
+        <v>0.92959391410953796</v>
+      </c>
+      <c r="C75" s="4"/>
       <c r="D75" s="4"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>11</v>
       </c>
-      <c r="B76" s="4">
+      <c r="B76" s="3">
+        <f>$D43/$B43</f>
         <v>0.95189771697377712</v>
       </c>
-      <c r="C76" s="4">
-        <v>0.91413733839426947</v>
-      </c>
+      <c r="C76" s="4"/>
       <c r="D76" s="4"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>12</v>
       </c>
-      <c r="B77" s="4">
+      <c r="B77" s="3">
+        <f>$D51/$B51</f>
         <v>0.8430629208604945</v>
       </c>
-      <c r="C77" s="4">
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="94.5" x14ac:dyDescent="0.5">
+      <c r="A81" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C81" s="2"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A82" t="s">
+        <v>18</v>
+      </c>
+      <c r="B82" s="3">
+        <f>$E7/$C7</f>
+        <v>0.49154000020318295</v>
+      </c>
+      <c r="C82" s="3"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A83" t="s">
+        <v>9</v>
+      </c>
+      <c r="B83" s="3">
+        <f>$E15/$C15</f>
+        <v>0.98361426054840106</v>
+      </c>
+      <c r="C83" s="4"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A84" t="s">
+        <v>8</v>
+      </c>
+      <c r="B84" s="3">
+        <f>$E25/$C25</f>
+        <v>0.90431492898636334</v>
+      </c>
+      <c r="C84" s="4"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A85" t="s">
+        <v>10</v>
+      </c>
+      <c r="B85" s="3">
+        <f>$E34/$C34</f>
+        <v>0.51917900623807023</v>
+      </c>
+      <c r="C85" s="4"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A86" t="s">
+        <v>11</v>
+      </c>
+      <c r="B86" s="3">
+        <f>$E43/$C43</f>
+        <v>0.91413733839426947</v>
+      </c>
+      <c r="C86" s="4"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A87" t="s">
+        <v>12</v>
+      </c>
+      <c r="B87" s="3">
+        <f>$E51/$C51</f>
         <v>0.72003049098828042</v>
       </c>
-      <c r="D77" s="4"/>
+      <c r="C87" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>